<commit_message>
fix local testing and udate test-data
</commit_message>
<xml_diff>
--- a/tools/facturation_ibps/test-data/testdouble.xlsx
+++ b/tools/facturation_ibps/test-data/testdouble.xlsx
@@ -3,165 +3,22 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="24300" windowWidth="34605" xWindow="14265" yWindow="4755"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="14265" yWindow="4755" windowWidth="34605" windowHeight="24300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="SMP-2011" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="152511" concurrentCalc="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511" fullCalcOnLoad="1" concurrentCalc="0"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
-  <si>
-    <t>Relevé de prestation de service - A REGLER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  imagerie-2018/ 217</t>
-  </si>
-  <si>
-    <t>référence à rappeler sur votre bon de commande</t>
-  </si>
-  <si>
-    <t>Siret: 130 023 385 00011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">période de la prestation: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8- 2018 </t>
-  </si>
-  <si>
-    <t>Coordonnées de la plateforme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordonnées du client </t>
-  </si>
-  <si>
-    <t>Adresse de l'appel Ã  facturation : UMR 7622 - S.Schneider-Maunoury</t>
-  </si>
-  <si>
-    <t>Institut de Biologie Paris-Seine - FR 3631</t>
-  </si>
-  <si>
-    <t>MorphogÃ©nÃ¨se du Cerveau des VertÃ©brÃ©s</t>
-  </si>
-  <si>
-    <t>IMAGERIE PHOTONIQUE</t>
-  </si>
-  <si>
-    <t>UniversitÃ© Pierre et Marie Curie</t>
-  </si>
-  <si>
-    <t>9 quai St Bernard - Bat B - 7è étage</t>
-  </si>
-  <si>
-    <t>9 Quai St Bernard</t>
-  </si>
-  <si>
-    <t>case courrier 24 - 75005 PARIS</t>
-  </si>
-  <si>
-    <t>Batiment C</t>
-  </si>
-  <si>
-    <t>7etage</t>
-  </si>
-  <si>
-    <t>Responsable: Susanne BOLTE</t>
-  </si>
-  <si>
-    <t>Paris</t>
-  </si>
-  <si>
-    <t>tel: 01 44 27 20 11</t>
-  </si>
-  <si>
-    <t>75005</t>
-  </si>
-  <si>
-    <t>mail: susanne.bolte@sorbonne-universite.fr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tel: </t>
-  </si>
-  <si>
-    <t>mail :</t>
-  </si>
-  <si>
-    <t>Gestionnaire tel: 01 44 27 58 89</t>
-  </si>
-  <si>
-    <t>Gestionnaire - tel:</t>
-  </si>
-  <si>
-    <t>mail: sciences-ibps-pf-recettes@sorbonne-universite.fr</t>
-  </si>
-  <si>
-    <t>mail:</t>
-  </si>
-  <si>
-    <t>Paris, le</t>
-  </si>
-  <si>
-    <t>20-09-2018</t>
-  </si>
-  <si>
-    <t>Désignation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantité (Heure) </t>
-  </si>
-  <si>
-    <t>Prix Unitaire</t>
-  </si>
-  <si>
-    <t>Montant HT</t>
-  </si>
-  <si>
-    <t>Confocal SP5 Droit 8-2018</t>
-  </si>
-  <si>
-    <t>77.00</t>
-  </si>
-  <si>
-    <t>21.00 â‚¬</t>
-  </si>
-  <si>
-    <t>Confocal SP5 InversÃ© 8-2018</t>
-  </si>
-  <si>
-    <t>14.00</t>
-  </si>
-  <si>
-    <t>Total Général HT</t>
-  </si>
-  <si>
-    <t>TVA 20%</t>
-  </si>
-  <si>
-    <t>Total Général TTC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce relevé est à régulariser par bon de commande* dans les 30 jours, par mail à                  sciences-ibps-pf-recettes@sorbonne-universite.fr  .                                                      </t>
-  </si>
-  <si>
-    <t>*Soit par bon de commande en Prestations Internes de Sorbonne Université. La plateforme est rattachée à la faculté des Sciences (budget).</t>
-  </si>
-  <si>
-    <t>*Soit par bon de commande externe (Cnrs, Inserm…etc) . Le bon doit être libellé au nom de Sorbonne Université</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt formatCode="#,##0.00\€;\-#,##0.00\€" numFmtId="164"/>
-    <numFmt formatCode="#,##0.00\ &quot;€&quot;" numFmtId="165"/>
-    <numFmt formatCode="_-* #,##0.00\ [$€]_-;\-* #,##0.00\ [$€]_-;_-* \-??\ [$€]_-;_-@_-" numFmtId="166"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\€;\-#,##0.00\€"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ [$€]_-;\-* #,##0.00\ [$€]_-;_-* \-??\ [$€]_-;_-@_-"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -349,7 +206,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -603,239 +460,277 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="166"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="11" numFmtId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="86">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="97">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="18" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="12" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="12" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="13" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="15" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="15" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="14" fillId="0" fontId="14" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="15" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="21" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="9" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="17" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="21" numFmtId="17" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="15" fillId="0" fontId="22" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="17" fontId="21" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="16" fillId="0" fontId="21" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="22" fillId="0" fontId="9" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="15" fillId="0" fontId="9" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="16" fillId="0" fontId="9" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="24" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="17" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="18" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="17" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="14" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="14" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="14" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="10" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="9" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="17" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="18" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="17" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="18" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="19" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="20" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="2" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="22" fillId="0" fontId="9" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="15" fillId="0" fontId="9" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="16" fillId="0" fontId="9" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Euro" xfId="1"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -851,7 +746,7 @@
     <ext cx="2381250" cy="923925"/>
     <pic>
       <nvPicPr>
-        <cNvPr descr="Picture" id="1" name="Image 1"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
@@ -1227,431 +1122,521 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.85546875" defaultRowHeight="12.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="13" width="43.7109375"/>
-    <col customWidth="1" max="2" min="2" style="13" width="6.7109375"/>
-    <col customWidth="1" max="3" min="3" style="13" width="6.42578125"/>
-    <col customWidth="1" max="4" min="4" style="13" width="15"/>
-    <col customWidth="1" max="5" min="5" style="13" width="21.42578125"/>
-    <col customWidth="1" max="16384" min="6" style="13" width="10.85546875"/>
+    <col width="43.7109375" customWidth="1" style="13" min="1" max="1"/>
+    <col width="6.7109375" customWidth="1" style="13" min="2" max="2"/>
+    <col width="6.42578125" customWidth="1" style="13" min="3" max="3"/>
+    <col width="15" customWidth="1" style="13" min="4" max="4"/>
+    <col width="21.42578125" customWidth="1" style="13" min="5" max="5"/>
+    <col width="10.85546875" customWidth="1" style="13" min="6" max="16384"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="24" r="1" s="35" spans="1:5">
+    <row r="1" ht="24" customHeight="1" s="35">
       <c r="A1" s="16" t="n"/>
-      <c r="B1" s="59" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="18" r="2" s="35" spans="1:5">
-      <c r="C2" s="66" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="3" s="35" spans="1:5">
-      <c r="C3" s="17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="B1" s="59" t="inlineStr">
+        <is>
+          <t>Relevé de prestation de service - A REGLER</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="18" customHeight="1" s="35">
+      <c r="C2" s="66" t="inlineStr">
+        <is>
+          <t>imagerie-2018/ 217</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1" s="35">
+      <c r="C3" s="17" t="inlineStr">
+        <is>
+          <t>référence à rappeler sur votre bon de commande</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="13" t="n"/>
     </row>
-    <row customHeight="1" ht="23.25" r="5" s="35" spans="1:5">
-      <c r="A5" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="52" t="s">
-        <v>4</v>
+    <row r="5" ht="23.25" customHeight="1" s="35">
+      <c r="A5" s="19" t="inlineStr">
+        <is>
+          <t>Siret: 130 023 385 00011</t>
+        </is>
+      </c>
+      <c r="C5" s="52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">période de la prestation: </t>
+        </is>
       </c>
       <c r="D5" s="52" t="n"/>
-      <c r="E5" s="49" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.5" r="6" s="35" spans="1:5" thickBot="1"/>
-    <row customHeight="1" ht="15.75" r="7" s="35" spans="1:5">
-      <c r="A7" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="63" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E5" s="49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">8- 2018 </t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="13.5" customHeight="1" s="35" thickBot="1"/>
+    <row r="7" ht="15.75" customHeight="1" s="35">
+      <c r="A7" s="32" t="inlineStr">
+        <is>
+          <t>Coordonnées de la plateforme</t>
+        </is>
+      </c>
+      <c r="C7" s="32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Coordonnées du client </t>
+        </is>
+      </c>
+      <c r="D7" s="80" t="n"/>
+      <c r="E7" s="81" t="n"/>
+    </row>
+    <row r="8">
       <c r="A8" s="31" t="n"/>
-      <c r="C8" s="40" t="s">
-        <v>8</v>
+      <c r="C8" s="40" t="inlineStr">
+        <is>
+          <t>UMR 7622 - S.Schneider-Maunoury</t>
+        </is>
       </c>
       <c r="D8" s="13" t="n"/>
       <c r="E8" s="27" t="n"/>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>10</v>
+    <row r="9">
+      <c r="A9" s="39" t="inlineStr">
+        <is>
+          <t>Institut de Biologie Paris-Seine - FR 3631</t>
+        </is>
+      </c>
+      <c r="C9" s="41" t="inlineStr">
+        <is>
+          <t>Morphogénèse du Cerveau des Vertébrés</t>
+        </is>
       </c>
       <c r="E9" s="27" t="n"/>
     </row>
-    <row customHeight="1" ht="18.75" r="10" s="35" spans="1:5">
-      <c r="A10" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="41" t="s">
-        <v>12</v>
+    <row r="10" ht="18.75" customHeight="1" s="35">
+      <c r="A10" s="50" t="inlineStr">
+        <is>
+          <t>IMAGERIE PHOTONIQUE</t>
+        </is>
+      </c>
+      <c r="C10" s="41" t="inlineStr">
+        <is>
+          <t>Université Pierre et Marie Curie</t>
+        </is>
       </c>
       <c r="E10" s="27" t="n"/>
     </row>
-    <row customHeight="1" ht="12.75" r="11" s="35" spans="1:5">
-      <c r="A11" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>14</v>
+    <row r="11" ht="12.75" customHeight="1" s="35">
+      <c r="A11" s="31" t="inlineStr">
+        <is>
+          <t>9 quai St Bernard - Bat B - 7è étage</t>
+        </is>
+      </c>
+      <c r="C11" s="41" t="inlineStr">
+        <is>
+          <t>9 Quai St Bernard</t>
+        </is>
       </c>
       <c r="E11" s="27" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="12" s="35" spans="1:5">
-      <c r="A12" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="41" t="s">
-        <v>16</v>
+    <row r="12" ht="15.75" customHeight="1" s="35">
+      <c r="A12" s="31" t="inlineStr">
+        <is>
+          <t>case courrier 24 - 75005 PARIS</t>
+        </is>
+      </c>
+      <c r="C12" s="41" t="inlineStr">
+        <is>
+          <t>Batiment C</t>
+        </is>
       </c>
       <c r="E12" s="28" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="13" s="35" spans="1:5">
+    <row r="13" ht="15.75" customHeight="1" s="35">
       <c r="A13" s="31" t="n"/>
-      <c r="C13" s="41" t="s">
-        <v>17</v>
+      <c r="C13" s="41" t="inlineStr">
+        <is>
+          <t>7etage</t>
+        </is>
       </c>
       <c r="E13" s="28" t="n"/>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="40" t="s">
-        <v>19</v>
+    <row r="14">
+      <c r="A14" s="31" t="inlineStr">
+        <is>
+          <t>Responsable: Susanne BOLTE</t>
+        </is>
+      </c>
+      <c r="C14" s="40" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
       </c>
       <c r="E14" s="28" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="15" s="35" spans="1:5">
-      <c r="A15" s="31" t="s">
-        <v>20</v>
+    <row r="15" ht="15.75" customHeight="1" s="35">
+      <c r="A15" s="31" t="inlineStr">
+        <is>
+          <t>tel: 01 44 27 20 11</t>
+        </is>
       </c>
       <c r="B15" s="26" t="n"/>
-      <c r="C15" s="40" t="s">
-        <v>21</v>
+      <c r="C15" s="40" t="inlineStr">
+        <is>
+          <t>75005</t>
+        </is>
       </c>
       <c r="E15" s="28" t="n"/>
     </row>
-    <row customHeight="1" ht="16.5" r="16" s="35" spans="1:5">
-      <c r="A16" s="39" t="s">
-        <v>22</v>
+    <row r="16" ht="16.5" customHeight="1" s="35">
+      <c r="A16" s="39" t="inlineStr">
+        <is>
+          <t>mail: susanne.bolte@sorbonne-universite.fr</t>
+        </is>
       </c>
       <c r="B16" s="24" t="n"/>
-      <c r="C16" s="41" t="s">
-        <v>23</v>
+      <c r="C16" s="41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tel: </t>
+        </is>
       </c>
       <c r="D16" s="52" t="n"/>
       <c r="E16" s="53" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="17" s="35" spans="1:5">
+    <row r="17" ht="15" customHeight="1" s="35">
       <c r="A17" s="31" t="n"/>
       <c r="B17" s="25" t="n"/>
-      <c r="C17" s="51" t="s">
-        <v>24</v>
+      <c r="C17" s="51" t="inlineStr">
+        <is>
+          <t>mail :</t>
+        </is>
       </c>
       <c r="D17" s="37" t="n"/>
       <c r="E17" s="28" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="18" s="35" spans="1:5">
-      <c r="A18" s="31" t="s">
-        <v>25</v>
+    <row r="18" ht="15" customHeight="1" s="35">
+      <c r="A18" s="31" t="inlineStr">
+        <is>
+          <t>Gestionnaire tel: 01 44 27 58 89</t>
+        </is>
       </c>
       <c r="B18" s="25" t="n"/>
-      <c r="C18" s="36" t="s">
-        <v>26</v>
+      <c r="C18" s="36" t="inlineStr">
+        <is>
+          <t>Gestionnaire - tel:</t>
+        </is>
       </c>
       <c r="D18" s="38" t="n"/>
       <c r="E18" s="28" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="19" s="35" spans="1:5" thickBot="1">
-      <c r="A19" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="42" t="s">
-        <v>28</v>
+    <row r="19" ht="15" customHeight="1" s="35" thickBot="1">
+      <c r="A19" s="55" t="inlineStr">
+        <is>
+          <t>mail: sciences-ibps-pf-recettes@sorbonne-universite.fr</t>
+        </is>
+      </c>
+      <c r="C19" s="42" t="inlineStr">
+        <is>
+          <t>mail:</t>
+        </is>
       </c>
       <c r="D19" s="43" t="n"/>
       <c r="E19" s="29" t="n"/>
     </row>
-    <row customHeight="1" ht="19.5" r="20" s="35" spans="1:5">
+    <row r="20" ht="19.5" customHeight="1" s="35">
       <c r="A20" s="62" t="n"/>
     </row>
-    <row customHeight="1" ht="19.5" r="21" s="35" spans="1:5">
+    <row r="21" ht="19.5" customHeight="1" s="35">
       <c r="A21" s="62" t="n"/>
       <c r="B21" s="62" t="n"/>
       <c r="C21" s="62" t="n"/>
-      <c r="D21" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="54" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="22" s="35" spans="1:5" thickBot="1">
+      <c r="D21" s="48" t="inlineStr">
+        <is>
+          <t>Paris, le</t>
+        </is>
+      </c>
+      <c r="E21" s="54" t="inlineStr">
+        <is>
+          <t>20-09-2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="15" customHeight="1" s="35" thickBot="1">
       <c r="A22" s="14" t="n"/>
       <c r="B22" s="14" t="n"/>
       <c r="C22" s="14" t="n"/>
       <c r="D22" s="14" t="n"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="32.25" r="23" s="3" spans="1:5" thickBot="1">
-      <c r="A23" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="68" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="18.75" r="24" s="3" spans="1:5">
+    <row r="23" ht="32.25" customFormat="1" customHeight="1" s="3" thickBot="1">
+      <c r="A23" s="44" t="inlineStr">
+        <is>
+          <t>Désignation</t>
+        </is>
+      </c>
+      <c r="B23" s="82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Quantité (Heure) </t>
+        </is>
+      </c>
+      <c r="C23" s="83" t="n"/>
+      <c r="D23" s="45" t="inlineStr">
+        <is>
+          <t>Prix Unitaire</t>
+        </is>
+      </c>
+      <c r="E23" s="68" t="inlineStr">
+        <is>
+          <t>Montant HT</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="18.75" customFormat="1" customHeight="1" s="3">
       <c r="A24" s="4" t="n">
         <v/>
       </c>
-      <c r="B24" s="69" t="n">
+      <c r="B24" s="84" t="n">
         <v/>
       </c>
-      <c r="D24" s="20" t="n">
+      <c r="C24" s="85" t="n"/>
+      <c r="D24" s="86" t="n">
         <v/>
       </c>
-      <c r="E24" s="80" t="n"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="20.1" r="25" s="3" spans="1:5">
-      <c r="A25" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="72" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="81">
-        <f>D25*B25</f>
-        <v/>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="20.1" r="26" s="3" spans="1:5">
-      <c r="A26" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="81">
-        <f>D26*B26</f>
-        <v/>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="20.1" r="27" s="3" spans="1:5">
+      <c r="E24" s="87" t="n"/>
+    </row>
+    <row r="25" ht="20.1" customFormat="1" customHeight="1" s="3">
+      <c r="A25" s="5" t="inlineStr">
+        <is>
+          <t>Confocal SP5 Droit 8-2018</t>
+        </is>
+      </c>
+      <c r="B25" s="88" t="n">
+        <v>77</v>
+      </c>
+      <c r="C25" s="85" t="n"/>
+      <c r="D25" s="88" t="n">
+        <v>21</v>
+      </c>
+      <c r="E25" s="89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" ht="20.1" customFormat="1" customHeight="1" s="3">
+      <c r="A26" s="7" t="inlineStr">
+        <is>
+          <t>Confocal SP5 Inversé 8-2018</t>
+        </is>
+      </c>
+      <c r="B26" s="90" t="n">
+        <v>14</v>
+      </c>
+      <c r="C26" s="85" t="n"/>
+      <c r="D26" s="90" t="n">
+        <v>21</v>
+      </c>
+      <c r="E26" s="89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" ht="20.1" customFormat="1" customHeight="1" s="3">
       <c r="A27" s="7" t="n"/>
-      <c r="B27" s="60" t="n"/>
+      <c r="B27" s="22" t="n"/>
+      <c r="C27" s="85" t="n"/>
       <c r="D27" s="22" t="n"/>
-      <c r="E27" s="81">
-        <f>D27*B27</f>
-        <v/>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="20.1" r="28" s="3" spans="1:5">
+      <c r="E27" s="89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" ht="20.1" customFormat="1" customHeight="1" s="3">
       <c r="A28" s="8" t="n"/>
-      <c r="B28" s="60" t="n"/>
+      <c r="B28" s="22" t="n"/>
+      <c r="C28" s="85" t="n"/>
       <c r="D28" s="21" t="n"/>
-      <c r="E28" s="81">
-        <f>D28*B28</f>
-        <v/>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="20.1" r="29" s="3" spans="1:5">
+      <c r="E28" s="89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" ht="20.1" customFormat="1" customHeight="1" s="3">
       <c r="A29" s="9" t="n"/>
-      <c r="B29" s="60" t="n"/>
+      <c r="B29" s="22" t="n"/>
+      <c r="C29" s="85" t="n"/>
       <c r="D29" s="21" t="n"/>
-      <c r="E29" s="81">
-        <f>D29*B29</f>
-        <v/>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="20.1" r="30" s="3" spans="1:5">
+      <c r="E29" s="89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" ht="20.1" customFormat="1" customHeight="1" s="3">
       <c r="A30" s="5" t="n"/>
-      <c r="B30" s="60" t="n"/>
+      <c r="B30" s="22" t="n"/>
+      <c r="C30" s="85" t="n"/>
       <c r="D30" s="21" t="n"/>
-      <c r="E30" s="81">
-        <f>D30*B30</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="20.1" r="31" s="35" spans="1:5">
+      <c r="E30" s="89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" ht="20.1" customHeight="1" s="35">
       <c r="A31" s="5" t="n"/>
-      <c r="B31" s="60" t="n"/>
+      <c r="B31" s="22" t="n"/>
+      <c r="C31" s="85" t="n"/>
       <c r="D31" s="21" t="n"/>
-      <c r="E31" s="81">
-        <f>D31*B31</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="20.1" r="32" s="35" spans="1:5">
+      <c r="E31" s="89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" ht="20.1" customHeight="1" s="35">
       <c r="A32" s="8" t="n"/>
-      <c r="B32" s="60" t="n"/>
+      <c r="B32" s="22" t="n"/>
+      <c r="C32" s="85" t="n"/>
       <c r="D32" s="21" t="n"/>
-      <c r="E32" s="81">
-        <f>D32*B32</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="20.1" r="33" s="35" spans="1:5">
+      <c r="E32" s="89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" ht="20.1" customHeight="1" s="35">
       <c r="A33" s="5" t="n"/>
-      <c r="B33" s="60" t="n"/>
+      <c r="B33" s="22" t="n"/>
+      <c r="C33" s="85" t="n"/>
       <c r="D33" s="21" t="n"/>
-      <c r="E33" s="81">
-        <f>D33*B33</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="20.1" r="34" s="35" spans="1:5">
+      <c r="E33" s="89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" ht="20.1" customHeight="1" s="35">
       <c r="A34" s="7" t="n"/>
-      <c r="B34" s="60" t="n"/>
+      <c r="B34" s="22" t="n"/>
+      <c r="C34" s="85" t="n"/>
       <c r="D34" s="21" t="n"/>
-      <c r="E34" s="81">
-        <f>D34*B34</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="20.1" r="35" s="35" spans="1:5">
+      <c r="E34" s="89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" ht="20.1" customHeight="1" s="35">
       <c r="A35" s="5" t="n"/>
-      <c r="B35" s="60" t="n"/>
+      <c r="B35" s="22" t="n"/>
+      <c r="C35" s="85" t="n"/>
       <c r="D35" s="21" t="n"/>
-      <c r="E35" s="81">
-        <f>D35*B35</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="20.1" r="36" s="35" spans="1:5" thickBot="1">
+      <c r="E35" s="89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" ht="20.1" customHeight="1" s="35" thickBot="1">
       <c r="A36" s="10" t="n"/>
-      <c r="B36" s="76" t="n"/>
+      <c r="B36" s="91" t="n"/>
+      <c r="C36" s="92" t="n"/>
       <c r="D36" s="23" t="n"/>
-      <c r="E36" s="82" t="n"/>
-    </row>
-    <row customHeight="1" ht="27" r="37" s="35" spans="1:5">
+      <c r="E36" s="93" t="n"/>
+    </row>
+    <row r="37" ht="27" customHeight="1" s="35">
       <c r="A37" s="79" t="n"/>
-      <c r="B37" s="78" t="s">
-        <v>40</v>
-      </c>
-      <c r="E37" s="83">
-        <f>SUM(E24:E36)</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="24" r="38" s="35" spans="1:5">
-      <c r="B38" s="74" t="s">
-        <v>41</v>
-      </c>
-      <c r="E38" s="84">
-        <f>E37*20%</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="24.75" r="39" s="35" spans="1:5" thickBot="1">
-      <c r="B39" s="74" t="s">
-        <v>42</v>
-      </c>
-      <c r="E39" s="85">
-        <f>E37+E38</f>
-        <v/>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="12.75" r="40" s="52" spans="1:5">
+      <c r="B37" s="78" t="inlineStr">
+        <is>
+          <t>Total Général HT</t>
+        </is>
+      </c>
+      <c r="C37" s="80" t="n"/>
+      <c r="D37" s="80" t="n"/>
+      <c r="E37" s="94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" ht="24" customHeight="1" s="35">
+      <c r="B38" s="74" t="inlineStr">
+        <is>
+          <t>TVA 20%</t>
+        </is>
+      </c>
+      <c r="E38" s="95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" ht="24.75" customHeight="1" s="35" thickBot="1">
+      <c r="B39" s="74" t="inlineStr">
+        <is>
+          <t>Total Général TTC</t>
+        </is>
+      </c>
+      <c r="E39" s="96" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" ht="12.75" customFormat="1" customHeight="1" s="52">
       <c r="B40" s="18" t="n"/>
       <c r="C40" s="18" t="n"/>
       <c r="D40" s="18" t="n"/>
     </row>
-    <row customHeight="1" ht="39.75" r="41" s="35" spans="1:5">
-      <c r="A41" s="75" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="26.25" r="42" s="35" spans="1:5">
-      <c r="A42" s="71" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="22.5" r="43" s="35" spans="1:5">
-      <c r="A43" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5"/>
-    <row r="45" spans="1:5"/>
-    <row r="46" spans="1:5"/>
-    <row r="47" spans="1:5"/>
-    <row r="48" spans="1:5"/>
-    <row r="49" spans="1:5"/>
-    <row r="50" spans="1:5"/>
-    <row r="51" spans="1:5"/>
-    <row r="52" spans="1:5"/>
-    <row r="53" spans="1:5"/>
-    <row r="54" spans="1:5"/>
-    <row r="55" spans="1:5"/>
-    <row r="56" spans="1:5"/>
-    <row r="57" spans="1:5"/>
-    <row r="58" spans="1:5"/>
-    <row r="59" spans="1:5"/>
-    <row r="60" spans="1:5"/>
-    <row r="61" spans="1:5"/>
-    <row r="62" spans="1:5"/>
-    <row r="63" spans="1:5"/>
-    <row r="64" spans="1:5"/>
-    <row r="65" spans="1:5"/>
-    <row r="66" spans="1:5"/>
-    <row r="67" spans="1:5"/>
-    <row r="68" spans="1:5"/>
-    <row r="69" spans="1:5"/>
-    <row r="70" spans="1:5"/>
-    <row r="71" spans="1:5"/>
-    <row r="72" spans="1:5"/>
-    <row r="73" spans="1:5"/>
-    <row r="74" spans="1:5"/>
-    <row r="75" spans="1:5"/>
-    <row r="76" spans="1:5"/>
-    <row r="77" spans="1:5"/>
-    <row r="78" spans="1:5"/>
-    <row r="79" spans="1:5"/>
-    <row r="80" spans="1:5"/>
-    <row r="81" spans="1:5"/>
-    <row r="82" spans="1:5"/>
-    <row r="83" spans="1:5"/>
-    <row r="84" spans="1:5"/>
-    <row r="85" spans="1:5"/>
-    <row r="86" spans="1:5"/>
-    <row r="87" spans="1:5"/>
-    <row r="88" spans="1:5"/>
-    <row r="89" spans="1:5"/>
-    <row r="90" spans="1:5"/>
-    <row r="91" spans="1:5"/>
-    <row r="92" spans="1:5"/>
-    <row r="93" spans="1:5"/>
-    <row r="94" spans="1:5"/>
-    <row r="95" spans="1:5"/>
-    <row r="96" spans="1:5"/>
+    <row r="41" ht="39.75" customHeight="1" s="35">
+      <c r="A41" s="75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ce relevé est à régulariser par bon de commande* dans les 30 jours, par mail à                  sciences-ibps-pf-recettes@sorbonne-universite.fr  .                                                      </t>
+        </is>
+      </c>
+    </row>
+    <row r="42" ht="26.25" customHeight="1" s="35">
+      <c r="A42" s="71" t="inlineStr">
+        <is>
+          <t>*Soit par bon de commande en Prestations Internes de Sorbonne Université. La plateforme est rattachée à la faculté des Sciences (budget).</t>
+        </is>
+      </c>
+    </row>
+    <row r="43" ht="22.5" customHeight="1" s="35">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>*Soit par bon de commande externe (Cnrs, Inserm…etc) . Le bon doit être libellé au nom de Sorbonne Université</t>
+        </is>
+      </c>
+    </row>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
   </sheetData>
   <mergeCells count="24">
     <mergeCell ref="A42:E42"/>
@@ -1680,8 +1665,8 @@
     <mergeCell ref="B24:C24"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins bottom="1.003125" footer="0.5118055555555555" header="0.5118055555555555" left="0.7875" right="0.7875" top="0.384375"/>
-  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="9" scale="90" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.384375" bottom="1.003125" header="0.5118055555555555" footer="0.5118055555555555"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="90" firstPageNumber="0" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
     <oddHeader/>
     <oddFooter>&amp;C&amp;K00-033Sorbonne Université_x000a_21, rue de l'Ecole de Médecine_x000a_75006 PARIS</oddFooter>

</xml_diff>

<commit_message>
fix bug in the python script and improve accuracy of tests
</commit_message>
<xml_diff>
--- a/tools/facturation_ibps/test-data/testdouble.xlsx
+++ b/tools/facturation_ibps/test-data/testdouble.xlsx
@@ -1796,8 +1796,9 @@
       <c r="D25" s="90" t="n">
         <v>21</v>
       </c>
-      <c r="E25" s="53" t="n">
-        <v>0</v>
+      <c r="E25" s="53">
+        <f>D25*B25</f>
+        <v/>
       </c>
       <c r="F25" s="44" t="n"/>
       <c r="G25" s="44" t="n"/>
@@ -1834,8 +1835,9 @@
       <c r="D26" s="91" t="n">
         <v>21</v>
       </c>
-      <c r="E26" s="53" t="n">
-        <v>0</v>
+      <c r="E26" s="53">
+        <f>D26*B26</f>
+        <v/>
       </c>
       <c r="F26" s="44" t="n"/>
       <c r="G26" s="44" t="n"/>
@@ -1864,8 +1866,9 @@
       <c r="B27" s="56" t="n"/>
       <c r="C27" s="88" t="n"/>
       <c r="D27" s="56" t="n"/>
-      <c r="E27" s="53" t="n">
-        <v>0</v>
+      <c r="E27" s="53">
+        <f>D27*B27</f>
+        <v/>
       </c>
       <c r="F27" s="44" t="n"/>
       <c r="G27" s="44" t="n"/>
@@ -1894,8 +1897,9 @@
       <c r="B28" s="56" t="n"/>
       <c r="C28" s="88" t="n"/>
       <c r="D28" s="52" t="n"/>
-      <c r="E28" s="53" t="n">
-        <v>0</v>
+      <c r="E28" s="53">
+        <f>D28*B28</f>
+        <v/>
       </c>
       <c r="F28" s="44" t="n"/>
       <c r="G28" s="44" t="n"/>
@@ -1924,8 +1928,9 @@
       <c r="B29" s="56" t="n"/>
       <c r="C29" s="88" t="n"/>
       <c r="D29" s="52" t="n"/>
-      <c r="E29" s="53" t="n">
-        <v>0</v>
+      <c r="E29" s="53">
+        <f>D29*B29</f>
+        <v/>
       </c>
       <c r="F29" s="44" t="n"/>
       <c r="G29" s="44" t="n"/>
@@ -1954,8 +1959,9 @@
       <c r="B30" s="56" t="n"/>
       <c r="C30" s="88" t="n"/>
       <c r="D30" s="52" t="n"/>
-      <c r="E30" s="53" t="n">
-        <v>0</v>
+      <c r="E30" s="53">
+        <f>D30*B30</f>
+        <v/>
       </c>
       <c r="F30" s="44" t="n"/>
       <c r="G30" s="44" t="n"/>
@@ -1984,8 +1990,9 @@
       <c r="B31" s="56" t="n"/>
       <c r="C31" s="88" t="n"/>
       <c r="D31" s="52" t="n"/>
-      <c r="E31" s="53" t="n">
-        <v>0</v>
+      <c r="E31" s="53">
+        <f>D31*B31</f>
+        <v/>
       </c>
       <c r="F31" s="3" t="n"/>
       <c r="G31" s="3" t="n"/>
@@ -2014,8 +2021,9 @@
       <c r="B32" s="56" t="n"/>
       <c r="C32" s="88" t="n"/>
       <c r="D32" s="52" t="n"/>
-      <c r="E32" s="53" t="n">
-        <v>0</v>
+      <c r="E32" s="53">
+        <f>D32*B32</f>
+        <v/>
       </c>
       <c r="F32" s="3" t="n"/>
       <c r="G32" s="3" t="n"/>
@@ -2044,8 +2052,9 @@
       <c r="B33" s="56" t="n"/>
       <c r="C33" s="88" t="n"/>
       <c r="D33" s="52" t="n"/>
-      <c r="E33" s="53" t="n">
-        <v>0</v>
+      <c r="E33" s="53">
+        <f>D33*B33</f>
+        <v/>
       </c>
       <c r="F33" s="3" t="n"/>
       <c r="G33" s="3" t="n"/>
@@ -2074,8 +2083,9 @@
       <c r="B34" s="56" t="n"/>
       <c r="C34" s="88" t="n"/>
       <c r="D34" s="52" t="n"/>
-      <c r="E34" s="53" t="n">
-        <v>0</v>
+      <c r="E34" s="53">
+        <f>D34*B34</f>
+        <v/>
       </c>
       <c r="F34" s="3" t="n"/>
       <c r="G34" s="3" t="n"/>
@@ -2104,8 +2114,9 @@
       <c r="B35" s="56" t="n"/>
       <c r="C35" s="88" t="n"/>
       <c r="D35" s="52" t="n"/>
-      <c r="E35" s="53" t="n">
-        <v>0</v>
+      <c r="E35" s="53">
+        <f>D35*B35</f>
+        <v/>
       </c>
       <c r="F35" s="3" t="n"/>
       <c r="G35" s="3" t="n"/>
@@ -2166,8 +2177,9 @@
       </c>
       <c r="C37" s="82" t="n"/>
       <c r="D37" s="82" t="n"/>
-      <c r="E37" s="68" t="n">
-        <v>0</v>
+      <c r="E37" s="68">
+        <f>SUM(E24:E36)</f>
+        <v/>
       </c>
       <c r="F37" s="3" t="n"/>
       <c r="G37" s="3" t="n"/>
@@ -2200,8 +2212,9 @@
       </c>
       <c r="C38" s="79" t="n"/>
       <c r="D38" s="79" t="n"/>
-      <c r="E38" s="72" t="n">
-        <v>0</v>
+      <c r="E38" s="72">
+        <f>E37*20%</f>
+        <v/>
       </c>
       <c r="F38" s="3" t="n"/>
       <c r="G38" s="3" t="n"/>
@@ -2234,8 +2247,9 @@
       </c>
       <c r="C39" s="79" t="n"/>
       <c r="D39" s="79" t="n"/>
-      <c r="E39" s="73" t="n">
-        <v>0</v>
+      <c r="E39" s="73">
+        <f>E37+E38</f>
+        <v/>
       </c>
       <c r="F39" s="3" t="n"/>
       <c r="G39" s="3" t="n"/>

</xml_diff>